<commit_message>
Mapping on 1km and 10km reference grids
</commit_message>
<xml_diff>
--- a/analysis/metadata/P12_5/P12_5_minimal_metadata.xlsx
+++ b/analysis/metadata/P12_5/P12_5_minimal_metadata.xlsx
@@ -4538,12 +4538,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C58">
-        <v>56.27638889</v>
-      </c>
-      <c r="D58">
-        <v>18.17055556</v>
-      </c>
       <c r="E58" t="inlineStr">
         <is>
           <t>marine</t>
@@ -4551,7 +4545,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -4596,7 +4590,7 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -4611,12 +4605,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C59">
-        <v>56.44305556</v>
-      </c>
-      <c r="D59">
-        <v>18.21</v>
-      </c>
       <c r="E59" t="inlineStr">
         <is>
           <t>marine</t>
@@ -4624,7 +4612,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -4669,7 +4657,7 @@
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7312,12 +7300,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C96">
-        <v>56.44305556</v>
-      </c>
-      <c r="D96">
-        <v>18.21</v>
-      </c>
       <c r="E96" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7325,7 +7307,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -7370,7 +7352,7 @@
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7385,12 +7367,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C97">
-        <v>56.44305556</v>
-      </c>
-      <c r="D97">
-        <v>18.21</v>
-      </c>
       <c r="E97" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7398,7 +7374,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -7443,7 +7419,7 @@
       </c>
       <c r="P97" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7458,12 +7434,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C98">
-        <v>56.44305556</v>
-      </c>
-      <c r="D98">
-        <v>18.21</v>
-      </c>
       <c r="E98" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7471,7 +7441,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -7516,7 +7486,7 @@
       </c>
       <c r="P98" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7531,12 +7501,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C99">
-        <v>56.44305556</v>
-      </c>
-      <c r="D99">
-        <v>18.21</v>
-      </c>
       <c r="E99" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7544,7 +7508,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -7589,7 +7553,7 @@
       </c>
       <c r="P99" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7604,12 +7568,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C100">
-        <v>56.44305556</v>
-      </c>
-      <c r="D100">
-        <v>18.21</v>
-      </c>
       <c r="E100" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7617,7 +7575,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -7662,7 +7620,7 @@
       </c>
       <c r="P100" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7677,12 +7635,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C101">
-        <v>56.44305556</v>
-      </c>
-      <c r="D101">
-        <v>18.21</v>
-      </c>
       <c r="E101" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7690,7 +7642,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -7735,7 +7687,7 @@
       </c>
       <c r="P101" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7750,12 +7702,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C102">
-        <v>56.44305556</v>
-      </c>
-      <c r="D102">
-        <v>18.21</v>
-      </c>
       <c r="E102" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7763,7 +7709,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -7808,7 +7754,7 @@
       </c>
       <c r="P102" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7823,12 +7769,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C103">
-        <v>56.44305556</v>
-      </c>
-      <c r="D103">
-        <v>18.21</v>
-      </c>
       <c r="E103" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7836,7 +7776,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -7881,7 +7821,7 @@
       </c>
       <c r="P103" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7896,12 +7836,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C104">
-        <v>56.44305556</v>
-      </c>
-      <c r="D104">
-        <v>18.21</v>
-      </c>
       <c r="E104" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7909,7 +7843,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -7954,7 +7888,7 @@
       </c>
       <c r="P104" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -7969,12 +7903,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C105">
-        <v>56.44305556</v>
-      </c>
-      <c r="D105">
-        <v>18.21</v>
-      </c>
       <c r="E105" t="inlineStr">
         <is>
           <t>marine</t>
@@ -7982,7 +7910,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -8027,7 +7955,7 @@
       </c>
       <c r="P105" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8042,12 +7970,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C106">
-        <v>56.44305556</v>
-      </c>
-      <c r="D106">
-        <v>18.21</v>
-      </c>
       <c r="E106" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8055,7 +7977,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -8100,7 +8022,7 @@
       </c>
       <c r="P106" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8115,12 +8037,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C107">
-        <v>56.44305556</v>
-      </c>
-      <c r="D107">
-        <v>18.21</v>
-      </c>
       <c r="E107" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8128,7 +8044,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -8173,7 +8089,7 @@
       </c>
       <c r="P107" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8188,12 +8104,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C108">
-        <v>56.44305556</v>
-      </c>
-      <c r="D108">
-        <v>18.21</v>
-      </c>
       <c r="E108" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8201,7 +8111,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -8246,7 +8156,7 @@
       </c>
       <c r="P108" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8261,12 +8171,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C109">
-        <v>56.44305556</v>
-      </c>
-      <c r="D109">
-        <v>18.21</v>
-      </c>
       <c r="E109" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8274,7 +8178,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -8319,7 +8223,7 @@
       </c>
       <c r="P109" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8334,12 +8238,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C110">
-        <v>56.11666667</v>
-      </c>
-      <c r="D110">
-        <v>17.62416667</v>
-      </c>
       <c r="E110" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8347,7 +8245,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -8392,7 +8290,7 @@
       </c>
       <c r="P110" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8407,12 +8305,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C111">
-        <v>56.11666667</v>
-      </c>
-      <c r="D111">
-        <v>17.62416667</v>
-      </c>
       <c r="E111" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8420,7 +8312,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -8465,7 +8357,7 @@
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8480,12 +8372,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C112">
-        <v>56.11666667</v>
-      </c>
-      <c r="D112">
-        <v>17.62416667</v>
-      </c>
       <c r="E112" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8493,7 +8379,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -8538,7 +8424,7 @@
       </c>
       <c r="P112" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8553,12 +8439,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C113">
-        <v>56.11666667</v>
-      </c>
-      <c r="D113">
-        <v>17.62416667</v>
-      </c>
       <c r="E113" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8566,7 +8446,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -8611,7 +8491,7 @@
       </c>
       <c r="P113" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8626,12 +8506,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C114">
-        <v>56.11666667</v>
-      </c>
-      <c r="D114">
-        <v>17.62416667</v>
-      </c>
       <c r="E114" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8639,7 +8513,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -8684,7 +8558,7 @@
       </c>
       <c r="P114" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8699,12 +8573,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C115">
-        <v>56.11666667</v>
-      </c>
-      <c r="D115">
-        <v>17.62416667</v>
-      </c>
       <c r="E115" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8712,7 +8580,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -8757,7 +8625,7 @@
       </c>
       <c r="P115" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8772,12 +8640,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C116">
-        <v>56.11666667</v>
-      </c>
-      <c r="D116">
-        <v>17.62416667</v>
-      </c>
       <c r="E116" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8785,7 +8647,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -8830,7 +8692,7 @@
       </c>
       <c r="P116" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8845,12 +8707,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C117">
-        <v>56.11666667</v>
-      </c>
-      <c r="D117">
-        <v>17.62416667</v>
-      </c>
       <c r="E117" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8858,7 +8714,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -8903,7 +8759,7 @@
       </c>
       <c r="P117" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8918,12 +8774,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C118">
-        <v>56.11666667</v>
-      </c>
-      <c r="D118">
-        <v>17.62416667</v>
-      </c>
       <c r="E118" t="inlineStr">
         <is>
           <t>marine</t>
@@ -8931,7 +8781,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -8976,7 +8826,7 @@
       </c>
       <c r="P118" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -8991,12 +8841,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C119">
-        <v>56.11666667</v>
-      </c>
-      <c r="D119">
-        <v>17.62416667</v>
-      </c>
       <c r="E119" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9004,7 +8848,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -9049,7 +8893,7 @@
       </c>
       <c r="P119" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9064,12 +8908,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C120">
-        <v>56.11666667</v>
-      </c>
-      <c r="D120">
-        <v>17.62416667</v>
-      </c>
       <c r="E120" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9077,7 +8915,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -9122,7 +8960,7 @@
       </c>
       <c r="P120" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9137,12 +8975,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C121">
-        <v>56.11666667</v>
-      </c>
-      <c r="D121">
-        <v>17.62416667</v>
-      </c>
       <c r="E121" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9150,7 +8982,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -9195,7 +9027,7 @@
       </c>
       <c r="P121" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9210,12 +9042,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C122">
-        <v>56.11666667</v>
-      </c>
-      <c r="D122">
-        <v>17.62416667</v>
-      </c>
       <c r="E122" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9223,7 +9049,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -9268,7 +9094,7 @@
       </c>
       <c r="P122" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9283,12 +9109,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C123">
-        <v>56.11666667</v>
-      </c>
-      <c r="D123">
-        <v>17.62416667</v>
-      </c>
       <c r="E123" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9296,7 +9116,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -9341,7 +9161,7 @@
       </c>
       <c r="P123" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9356,12 +9176,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C124">
-        <v>56.13722222</v>
-      </c>
-      <c r="D124">
-        <v>17.62916667</v>
-      </c>
       <c r="E124" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9369,7 +9183,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -9414,7 +9228,7 @@
       </c>
       <c r="P124" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9429,12 +9243,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C125">
-        <v>56.51611111</v>
-      </c>
-      <c r="D125">
-        <v>18.3125</v>
-      </c>
       <c r="E125" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9442,7 +9250,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
@@ -9487,7 +9295,7 @@
       </c>
       <c r="P125" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9502,12 +9310,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C126">
-        <v>56.51611111</v>
-      </c>
-      <c r="D126">
-        <v>18.3125</v>
-      </c>
       <c r="E126" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9515,7 +9317,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -9560,7 +9362,7 @@
       </c>
       <c r="P126" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9575,12 +9377,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C127">
-        <v>56.51611111</v>
-      </c>
-      <c r="D127">
-        <v>18.3125</v>
-      </c>
       <c r="E127" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9588,7 +9384,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -9633,7 +9429,7 @@
       </c>
       <c r="P127" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9648,12 +9444,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C128">
-        <v>56.51611111</v>
-      </c>
-      <c r="D128">
-        <v>18.3125</v>
-      </c>
       <c r="E128" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9661,7 +9451,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
@@ -9706,7 +9496,7 @@
       </c>
       <c r="P128" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9721,12 +9511,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C129">
-        <v>56.51611111</v>
-      </c>
-      <c r="D129">
-        <v>18.3125</v>
-      </c>
       <c r="E129" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9734,7 +9518,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
@@ -9779,7 +9563,7 @@
       </c>
       <c r="P129" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9794,12 +9578,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C130">
-        <v>56.51611111</v>
-      </c>
-      <c r="D130">
-        <v>18.3125</v>
-      </c>
       <c r="E130" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9807,7 +9585,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -9852,7 +9630,7 @@
       </c>
       <c r="P130" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9867,12 +9645,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C131">
-        <v>56.51611111</v>
-      </c>
-      <c r="D131">
-        <v>18.3125</v>
-      </c>
       <c r="E131" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9880,7 +9652,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
@@ -9925,7 +9697,7 @@
       </c>
       <c r="P131" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -9940,12 +9712,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C132">
-        <v>56.51611111</v>
-      </c>
-      <c r="D132">
-        <v>18.3125</v>
-      </c>
       <c r="E132" t="inlineStr">
         <is>
           <t>marine</t>
@@ -9953,7 +9719,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -9998,7 +9764,7 @@
       </c>
       <c r="P132" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10013,12 +9779,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C133">
-        <v>56.51611111</v>
-      </c>
-      <c r="D133">
-        <v>18.3125</v>
-      </c>
       <c r="E133" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10026,7 +9786,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -10071,7 +9831,7 @@
       </c>
       <c r="P133" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10086,12 +9846,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C134">
-        <v>56.51611111</v>
-      </c>
-      <c r="D134">
-        <v>18.3125</v>
-      </c>
       <c r="E134" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10099,7 +9853,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -10144,7 +9898,7 @@
       </c>
       <c r="P134" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10159,12 +9913,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C135">
-        <v>56.51611111</v>
-      </c>
-      <c r="D135">
-        <v>18.3125</v>
-      </c>
       <c r="E135" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10172,7 +9920,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -10217,7 +9965,7 @@
       </c>
       <c r="P135" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10232,12 +9980,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C136">
-        <v>56.51611111</v>
-      </c>
-      <c r="D136">
-        <v>18.3125</v>
-      </c>
       <c r="E136" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10245,7 +9987,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -10290,7 +10032,7 @@
       </c>
       <c r="P136" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10305,12 +10047,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C137">
-        <v>56.51611111</v>
-      </c>
-      <c r="D137">
-        <v>18.3125</v>
-      </c>
       <c r="E137" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10318,7 +10054,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -10363,7 +10099,7 @@
       </c>
       <c r="P137" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10378,12 +10114,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C138">
-        <v>56.51611111</v>
-      </c>
-      <c r="D138">
-        <v>18.3125</v>
-      </c>
       <c r="E138" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10391,7 +10121,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -10436,7 +10166,7 @@
       </c>
       <c r="P138" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10451,12 +10181,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C139">
-        <v>56.13722222</v>
-      </c>
-      <c r="D139">
-        <v>17.62916667</v>
-      </c>
       <c r="E139" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10464,7 +10188,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -10509,7 +10233,7 @@
       </c>
       <c r="P139" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10524,12 +10248,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C140">
-        <v>56.13722222</v>
-      </c>
-      <c r="D140">
-        <v>17.62916667</v>
-      </c>
       <c r="E140" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10537,7 +10255,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -10582,7 +10300,7 @@
       </c>
       <c r="P140" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10597,12 +10315,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C141">
-        <v>56.13722222</v>
-      </c>
-      <c r="D141">
-        <v>17.62916667</v>
-      </c>
       <c r="E141" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10610,7 +10322,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
@@ -10655,7 +10367,7 @@
       </c>
       <c r="P141" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10670,12 +10382,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C142">
-        <v>56.13722222</v>
-      </c>
-      <c r="D142">
-        <v>17.62916667</v>
-      </c>
       <c r="E142" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10683,7 +10389,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -10728,7 +10434,7 @@
       </c>
       <c r="P142" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10743,12 +10449,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C143">
-        <v>56.13722222</v>
-      </c>
-      <c r="D143">
-        <v>17.62916667</v>
-      </c>
       <c r="E143" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10756,7 +10456,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -10801,7 +10501,7 @@
       </c>
       <c r="P143" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10816,12 +10516,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C144">
-        <v>56.13722222</v>
-      </c>
-      <c r="D144">
-        <v>17.62916667</v>
-      </c>
       <c r="E144" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10829,7 +10523,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -10874,7 +10568,7 @@
       </c>
       <c r="P144" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10889,12 +10583,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C145">
-        <v>56.13722222</v>
-      </c>
-      <c r="D145">
-        <v>17.62916667</v>
-      </c>
       <c r="E145" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10902,7 +10590,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -10947,7 +10635,7 @@
       </c>
       <c r="P145" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -10962,12 +10650,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C146">
-        <v>56.13722222</v>
-      </c>
-      <c r="D146">
-        <v>17.62916667</v>
-      </c>
       <c r="E146" t="inlineStr">
         <is>
           <t>marine</t>
@@ -10975,7 +10657,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -11020,7 +10702,7 @@
       </c>
       <c r="P146" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -11035,12 +10717,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C147">
-        <v>56.13722222</v>
-      </c>
-      <c r="D147">
-        <v>17.62916667</v>
-      </c>
       <c r="E147" t="inlineStr">
         <is>
           <t>marine</t>
@@ -11048,7 +10724,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -11093,7 +10769,7 @@
       </c>
       <c r="P147" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -11108,12 +10784,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C148">
-        <v>56.13722222</v>
-      </c>
-      <c r="D148">
-        <v>17.62916667</v>
-      </c>
       <c r="E148" t="inlineStr">
         <is>
           <t>marine</t>
@@ -11121,7 +10791,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
@@ -11166,7 +10836,7 @@
       </c>
       <c r="P148" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -11181,12 +10851,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C149">
-        <v>56.13722222</v>
-      </c>
-      <c r="D149">
-        <v>17.62916667</v>
-      </c>
       <c r="E149" t="inlineStr">
         <is>
           <t>marine</t>
@@ -11194,7 +10858,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
@@ -11239,7 +10903,7 @@
       </c>
       <c r="P149" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -11254,12 +10918,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C150">
-        <v>56.13722222</v>
-      </c>
-      <c r="D150">
-        <v>17.62916667</v>
-      </c>
       <c r="E150" t="inlineStr">
         <is>
           <t>marine</t>
@@ -11267,7 +10925,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -11312,7 +10970,7 @@
       </c>
       <c r="P150" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -11327,12 +10985,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C151">
-        <v>56.13722222</v>
-      </c>
-      <c r="D151">
-        <v>17.62916667</v>
-      </c>
       <c r="E151" t="inlineStr">
         <is>
           <t>marine</t>
@@ -11340,7 +10992,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -11385,7 +11037,7 @@
       </c>
       <c r="P151" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -11400,12 +11052,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C152">
-        <v>56.25916667</v>
-      </c>
-      <c r="D152">
-        <v>17.75944444</v>
-      </c>
       <c r="E152" t="inlineStr">
         <is>
           <t>marine</t>
@@ -11413,7 +11059,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -11458,7 +11104,7 @@
       </c>
       <c r="P152" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -11473,12 +11119,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C153">
-        <v>56.13722222</v>
-      </c>
-      <c r="D153">
-        <v>17.62916667</v>
-      </c>
       <c r="E153" t="inlineStr">
         <is>
           <t>marine</t>
@@ -11486,7 +11126,7 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
@@ -11531,7 +11171,7 @@
       </c>
       <c r="P153" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -15926,12 +15566,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C214">
-        <v>56.27638889</v>
-      </c>
-      <c r="D214">
-        <v>18.17055556</v>
-      </c>
       <c r="E214" t="inlineStr">
         <is>
           <t>marine</t>
@@ -15939,7 +15573,7 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -15984,7 +15618,7 @@
       </c>
       <c r="P214" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -15999,12 +15633,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C215">
-        <v>56.27638889</v>
-      </c>
-      <c r="D215">
-        <v>18.17055556</v>
-      </c>
       <c r="E215" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16012,7 +15640,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -16057,7 +15685,7 @@
       </c>
       <c r="P215" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16072,12 +15700,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C216">
-        <v>56.27638889</v>
-      </c>
-      <c r="D216">
-        <v>18.17055556</v>
-      </c>
       <c r="E216" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16085,7 +15707,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -16130,7 +15752,7 @@
       </c>
       <c r="P216" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16145,12 +15767,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C217">
-        <v>56.27638889</v>
-      </c>
-      <c r="D217">
-        <v>18.17055556</v>
-      </c>
       <c r="E217" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16158,7 +15774,7 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
@@ -16203,7 +15819,7 @@
       </c>
       <c r="P217" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16218,12 +15834,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C218">
-        <v>56.27638889</v>
-      </c>
-      <c r="D218">
-        <v>18.17055556</v>
-      </c>
       <c r="E218" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16231,7 +15841,7 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
@@ -16276,7 +15886,7 @@
       </c>
       <c r="P218" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16291,12 +15901,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C219">
-        <v>56.27638889</v>
-      </c>
-      <c r="D219">
-        <v>18.17055556</v>
-      </c>
       <c r="E219" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16304,7 +15908,7 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
@@ -16349,7 +15953,7 @@
       </c>
       <c r="P219" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16364,12 +15968,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C220">
-        <v>56.27638889</v>
-      </c>
-      <c r="D220">
-        <v>18.17055556</v>
-      </c>
       <c r="E220" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16377,7 +15975,7 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
@@ -16422,7 +16020,7 @@
       </c>
       <c r="P220" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16437,12 +16035,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C221">
-        <v>56.27638889</v>
-      </c>
-      <c r="D221">
-        <v>18.17055556</v>
-      </c>
       <c r="E221" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16450,7 +16042,7 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
@@ -16495,7 +16087,7 @@
       </c>
       <c r="P221" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16510,12 +16102,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C222">
-        <v>56.27638889</v>
-      </c>
-      <c r="D222">
-        <v>18.17055556</v>
-      </c>
       <c r="E222" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16523,7 +16109,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
@@ -16568,7 +16154,7 @@
       </c>
       <c r="P222" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16583,12 +16169,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C223">
-        <v>56.27638889</v>
-      </c>
-      <c r="D223">
-        <v>18.17055556</v>
-      </c>
       <c r="E223" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16596,7 +16176,7 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -16641,7 +16221,7 @@
       </c>
       <c r="P223" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16656,12 +16236,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C224">
-        <v>56.27638889</v>
-      </c>
-      <c r="D224">
-        <v>18.17055556</v>
-      </c>
       <c r="E224" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16669,7 +16243,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
@@ -16714,7 +16288,7 @@
       </c>
       <c r="P224" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16729,12 +16303,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C225">
-        <v>56.27638889</v>
-      </c>
-      <c r="D225">
-        <v>18.17055556</v>
-      </c>
       <c r="E225" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16742,7 +16310,7 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
@@ -16787,7 +16355,7 @@
       </c>
       <c r="P225" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16802,12 +16370,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C226">
-        <v>56.27638889</v>
-      </c>
-      <c r="D226">
-        <v>18.17055556</v>
-      </c>
       <c r="E226" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16815,7 +16377,7 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
@@ -16860,7 +16422,7 @@
       </c>
       <c r="P226" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -16875,12 +16437,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C227">
-        <v>56.27638889</v>
-      </c>
-      <c r="D227">
-        <v>18.17055556</v>
-      </c>
       <c r="E227" t="inlineStr">
         <is>
           <t>marine</t>
@@ -16888,7 +16444,7 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
@@ -16933,7 +16489,7 @@
       </c>
       <c r="P227" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -17824,12 +17380,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C240">
-        <v>56.25916667</v>
-      </c>
-      <c r="D240">
-        <v>17.75944444</v>
-      </c>
       <c r="E240" t="inlineStr">
         <is>
           <t>marine</t>
@@ -17837,7 +17387,7 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
@@ -17882,7 +17432,7 @@
       </c>
       <c r="P240" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -17897,12 +17447,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C241">
-        <v>56.25916667</v>
-      </c>
-      <c r="D241">
-        <v>17.75944444</v>
-      </c>
       <c r="E241" t="inlineStr">
         <is>
           <t>marine</t>
@@ -17910,7 +17454,7 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -17955,7 +17499,7 @@
       </c>
       <c r="P241" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -17970,12 +17514,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C242">
-        <v>56.25916667</v>
-      </c>
-      <c r="D242">
-        <v>17.75944444</v>
-      </c>
       <c r="E242" t="inlineStr">
         <is>
           <t>marine</t>
@@ -17983,7 +17521,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -18028,7 +17566,7 @@
       </c>
       <c r="P242" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18043,12 +17581,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C243">
-        <v>56.25916667</v>
-      </c>
-      <c r="D243">
-        <v>17.75944444</v>
-      </c>
       <c r="E243" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18056,7 +17588,7 @@
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -18101,7 +17633,7 @@
       </c>
       <c r="P243" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18116,12 +17648,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C244">
-        <v>56.25916667</v>
-      </c>
-      <c r="D244">
-        <v>17.75944444</v>
-      </c>
       <c r="E244" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18129,7 +17655,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -18174,7 +17700,7 @@
       </c>
       <c r="P244" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18189,12 +17715,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C245">
-        <v>56.25916667</v>
-      </c>
-      <c r="D245">
-        <v>17.75944444</v>
-      </c>
       <c r="E245" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18202,7 +17722,7 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G245" t="inlineStr">
@@ -18247,7 +17767,7 @@
       </c>
       <c r="P245" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18262,12 +17782,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C246">
-        <v>56.25916667</v>
-      </c>
-      <c r="D246">
-        <v>17.75944444</v>
-      </c>
       <c r="E246" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18275,7 +17789,7 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
@@ -18320,7 +17834,7 @@
       </c>
       <c r="P246" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18335,12 +17849,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C247">
-        <v>56.25916667</v>
-      </c>
-      <c r="D247">
-        <v>17.75944444</v>
-      </c>
       <c r="E247" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18348,7 +17856,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -18393,7 +17901,7 @@
       </c>
       <c r="P247" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18408,12 +17916,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C248">
-        <v>56.25916667</v>
-      </c>
-      <c r="D248">
-        <v>17.75944444</v>
-      </c>
       <c r="E248" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18421,7 +17923,7 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
@@ -18466,7 +17968,7 @@
       </c>
       <c r="P248" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18481,12 +17983,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C249">
-        <v>56.25916667</v>
-      </c>
-      <c r="D249">
-        <v>17.75944444</v>
-      </c>
       <c r="E249" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18494,7 +17990,7 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G249" t="inlineStr">
@@ -18539,7 +18035,7 @@
       </c>
       <c r="P249" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18554,12 +18050,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C250">
-        <v>56.25916667</v>
-      </c>
-      <c r="D250">
-        <v>17.75944444</v>
-      </c>
       <c r="E250" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18567,7 +18057,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
@@ -18612,7 +18102,7 @@
       </c>
       <c r="P250" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18627,12 +18117,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C251">
-        <v>56.25916667</v>
-      </c>
-      <c r="D251">
-        <v>17.75944444</v>
-      </c>
       <c r="E251" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18640,7 +18124,7 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G251" t="inlineStr">
@@ -18685,7 +18169,7 @@
       </c>
       <c r="P251" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18700,12 +18184,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C252">
-        <v>56.25916667</v>
-      </c>
-      <c r="D252">
-        <v>17.75944444</v>
-      </c>
       <c r="E252" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18713,7 +18191,7 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
@@ -18758,7 +18236,7 @@
       </c>
       <c r="P252" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -18773,12 +18251,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C253">
-        <v>56.25916667</v>
-      </c>
-      <c r="D253">
-        <v>17.75944444</v>
-      </c>
       <c r="E253" t="inlineStr">
         <is>
           <t>marine</t>
@@ -18786,7 +18258,7 @@
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G253" t="inlineStr">
@@ -18831,7 +18303,7 @@
       </c>
       <c r="P253" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -19284,12 +18756,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C260">
-        <v>56.11666667</v>
-      </c>
-      <c r="D260">
-        <v>17.62416667</v>
-      </c>
       <c r="E260" t="inlineStr">
         <is>
           <t>marine</t>
@@ -19297,7 +18763,7 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
@@ -19342,7 +18808,7 @@
       </c>
       <c r="P260" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -19576,12 +19042,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C264">
-        <v>56.51611111</v>
-      </c>
-      <c r="D264">
-        <v>18.3125</v>
-      </c>
       <c r="E264" t="inlineStr">
         <is>
           <t>marine</t>
@@ -19589,7 +19049,7 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G264" t="inlineStr">
@@ -19634,7 +19094,7 @@
       </c>
       <c r="P264" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -19649,12 +19109,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C265">
-        <v>56.13722222</v>
-      </c>
-      <c r="D265">
-        <v>17.62916667</v>
-      </c>
       <c r="E265" t="inlineStr">
         <is>
           <t>marine</t>
@@ -19662,7 +19116,7 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G265" t="inlineStr">
@@ -19707,7 +19161,7 @@
       </c>
       <c r="P265" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -19722,12 +19176,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C266">
-        <v>56.13722222</v>
-      </c>
-      <c r="D266">
-        <v>17.62916667</v>
-      </c>
       <c r="E266" t="inlineStr">
         <is>
           <t>marine</t>
@@ -19735,7 +19183,7 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G266" t="inlineStr">
@@ -19780,7 +19228,7 @@
       </c>
       <c r="P266" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -19795,12 +19243,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C267">
-        <v>56.27638889</v>
-      </c>
-      <c r="D267">
-        <v>18.17055556</v>
-      </c>
       <c r="E267" t="inlineStr">
         <is>
           <t>marine</t>
@@ -19808,7 +19250,7 @@
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
@@ -19853,7 +19295,7 @@
       </c>
       <c r="P267" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -19868,12 +19310,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C268">
-        <v>56.27638889</v>
-      </c>
-      <c r="D268">
-        <v>18.17055556</v>
-      </c>
       <c r="E268" t="inlineStr">
         <is>
           <t>marine</t>
@@ -19881,7 +19317,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -19926,7 +19362,7 @@
       </c>
       <c r="P268" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -20598,12 +20034,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C278">
-        <v>56.51611111</v>
-      </c>
-      <c r="D278">
-        <v>18.3125</v>
-      </c>
       <c r="E278" t="inlineStr">
         <is>
           <t>marine</t>
@@ -20611,7 +20041,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -20656,7 +20086,7 @@
       </c>
       <c r="P278" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -20671,12 +20101,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C279">
-        <v>56.51611111</v>
-      </c>
-      <c r="D279">
-        <v>18.3125</v>
-      </c>
       <c r="E279" t="inlineStr">
         <is>
           <t>marine</t>
@@ -20684,7 +20108,7 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
@@ -20729,7 +20153,7 @@
       </c>
       <c r="P279" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -21985,12 +21409,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C297">
-        <v>56.25916667</v>
-      </c>
-      <c r="D297">
-        <v>17.75944444</v>
-      </c>
       <c r="E297" t="inlineStr">
         <is>
           <t>marine</t>
@@ -21998,7 +21416,7 @@
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
@@ -22043,7 +21461,7 @@
       </c>
       <c r="P297" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>
@@ -22058,12 +21476,6 @@
           <t>sediment</t>
         </is>
       </c>
-      <c r="C298">
-        <v>56.25916667</v>
-      </c>
-      <c r="D298">
-        <v>17.75944444</v>
-      </c>
       <c r="E298" t="inlineStr">
         <is>
           <t>marine</t>
@@ -22071,7 +21483,7 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>1211</t>
+          <t>1210</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
@@ -22116,7 +21528,7 @@
       </c>
       <c r="P298" t="inlineStr">
         <is>
-          <t>Østersøen, Sweden</t>
+          <t>Østersøen</t>
         </is>
       </c>
     </row>

</xml_diff>